<commit_message>
V1.1 with leanier pandas code and README
</commit_message>
<xml_diff>
--- a/master_data/scoring top2020.xlsx
+++ b/master_data/scoring top2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex-perso/dev/top2020_riff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A30B5FE-2768-4745-9025-3FD2CE686432}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD948055-ED85-9A4F-B919-B565A4879B9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3558,9 +3558,9 @@
   </sheetPr>
   <dimension ref="A1:AG67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z64" sqref="Z64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6525,7 +6525,7 @@
     <row r="41" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4">
         <f ca="1">TODAY()</f>
-        <v>44205</v>
+        <v>44210</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>671</v>

</xml_diff>